<commit_message>
fix merging of C02 DATSETS and graph output.
</commit_message>
<xml_diff>
--- a/C02 Nature Paper.xlsx
+++ b/C02 Nature Paper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tranetechnologies-my.sharepoint.com/personal/declan_tannian_tranetechnologies_com/Documents/Desktop/Programming-for-Data-Analysis-Project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{7FE9B86E-9142-4271-91F3-2359E26192C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B63C13CA-D6E6-444B-A1FD-D2F7B6A54B53}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{7FE9B86E-9142-4271-91F3-2359E26192C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11195F95-E48F-442D-B526-CDE4437F8076}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.  new CO2 data" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,20 @@
     <sheet name="3.  Composite CO2" sheetId="4" r:id="rId3"/>
     <sheet name="Fig 1.  800 kyr of CO2" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="101716"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 

</xml_diff>